<commit_message>
change YCbCr from 5 bit to 8 bit
</commit_message>
<xml_diff>
--- a/scripts/YCbCrcalculator.xlsx
+++ b/scripts/YCbCrcalculator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tests\AlexVideo\TxRx\D0711\scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tests\AlexVideo\TxRx\D0911A\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A75FD7E-2C79-49FF-A6A4-935FCF7E880E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DADC9A5C-42A9-42C8-AFD2-0F29ACB43FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29010" yWindow="420" windowWidth="28800" windowHeight="15075" activeTab="1" xr2:uid="{0E92F24A-9A72-411F-A4AA-3DEDFFA6C1B2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0E92F24A-9A72-411F-A4AA-3DEDFFA6C1B2}"/>
   </bookViews>
   <sheets>
     <sheet name="RGB2YCbCr&amp;BK" sheetId="6" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="120">
   <si>
     <t>R</t>
   </si>
@@ -403,29 +403,14 @@
     <t>Gh</t>
   </si>
   <si>
-    <t>1F</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
+    <t>F8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -440,6 +425,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="177"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -968,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97090DF3-BB24-4F34-9F73-6D280FDB1221}">
   <dimension ref="A1:AM27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1473,36 +1465,36 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="C11">
-        <v>255</v>
+        <v>8</v>
       </c>
       <c r="D11">
-        <v>255</v>
+        <v>8</v>
       </c>
       <c r="H11" t="s">
         <v>9</v>
       </c>
       <c r="J11">
         <f>G19</f>
-        <v>128</v>
+        <v>248</v>
       </c>
       <c r="K11">
         <f>G19</f>
-        <v>128</v>
+        <v>248</v>
       </c>
       <c r="L11">
         <f>G18</f>
-        <v>128</v>
+        <v>87</v>
       </c>
       <c r="M11">
         <f>G18</f>
-        <v>128</v>
+        <v>87</v>
       </c>
       <c r="N11">
         <f>G17</f>
-        <v>255</v>
+        <v>80</v>
       </c>
       <c r="T11" t="s">
         <v>9</v>
@@ -1531,35 +1523,35 @@
     <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <f>DEC2HEX(B11)</f>
-        <v>FF</v>
+        <v>F8</v>
       </c>
       <c r="C12" t="str">
         <f>DEC2HEX(C11)</f>
-        <v>FF</v>
+        <v>8</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" ref="D12" si="7">DEC2HEX(D11)</f>
-        <v>FF</v>
+        <v>8</v>
       </c>
       <c r="J12" t="str">
         <f>DEC2HEX(J11)</f>
-        <v>80</v>
+        <v>F8</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" ref="K12:N12" si="8">DEC2HEX(K11)</f>
-        <v>80</v>
+        <v>F8</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="8"/>
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" si="8"/>
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="N12" t="str">
         <f t="shared" si="8"/>
-        <v>FF</v>
+        <v>50</v>
       </c>
       <c r="V12" t="str">
         <f>DEC2HEX(V11)</f>
@@ -1585,23 +1577,23 @@
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="J13">
         <f>J11-$F$2</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="K13">
         <f>K11-$F$2</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="L13">
         <f>L11-$F$2</f>
-        <v>0</v>
+        <v>-41</v>
       </c>
       <c r="M13">
         <f>M11-$F$2</f>
-        <v>0</v>
+        <v>-41</v>
       </c>
       <c r="N13">
         <f>N11</f>
-        <v>255</v>
+        <v>80</v>
       </c>
       <c r="V13">
         <f>V11-$F$2</f>
@@ -1627,23 +1619,23 @@
     <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="J14" t="str">
         <f>DEC2HEX(J13)</f>
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" ref="K14:N14" si="10">DEC2HEX(K13)</f>
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>FFFFFFFFD7</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>FFFFFFFFD7</v>
       </c>
       <c r="N14" t="str">
         <f t="shared" si="10"/>
-        <v>FF</v>
+        <v>50</v>
       </c>
       <c r="V14" t="str">
         <f>DEC2HEX(V13)</f>
@@ -1713,27 +1705,27 @@
       </c>
       <c r="B17">
         <f t="shared" ref="B17:D19" si="12">B$11*B6</f>
-        <v>19635</v>
+        <v>19096</v>
       </c>
       <c r="C17">
         <f t="shared" si="12"/>
-        <v>7395</v>
+        <v>232</v>
       </c>
       <c r="D17">
         <f t="shared" si="12"/>
-        <v>38250</v>
+        <v>1200</v>
       </c>
       <c r="E17">
         <f>SUM(B17:D17)</f>
-        <v>65280</v>
+        <v>20528</v>
       </c>
       <c r="F17">
         <f>INT(E17/$F$1)</f>
-        <v>255</v>
+        <v>80</v>
       </c>
       <c r="G17">
         <f>F17</f>
-        <v>255</v>
+        <v>80</v>
       </c>
       <c r="I17" t="s">
         <v>1</v>
@@ -1744,7 +1736,7 @@
       </c>
       <c r="K17">
         <f t="shared" ref="K17:N17" si="13">K$13*K6</f>
-        <v>0</v>
+        <v>-21960</v>
       </c>
       <c r="L17">
         <f t="shared" si="13"/>
@@ -1752,23 +1744,23 @@
       </c>
       <c r="M17">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>3608</v>
       </c>
       <c r="N17">
         <f t="shared" si="13"/>
-        <v>65280</v>
+        <v>20480</v>
       </c>
       <c r="O17">
         <f>SUM(J17:N17)</f>
-        <v>65280</v>
+        <v>2128</v>
       </c>
       <c r="P17">
         <f>INT(O17/$F$1)</f>
-        <v>255</v>
+        <v>8</v>
       </c>
       <c r="Q17">
         <f>IF(P17&gt;($F$1-2),$F$1-1,IF(P17&lt;0,0,P17))</f>
-        <v>255</v>
+        <v>8</v>
       </c>
       <c r="R17" t="s">
         <v>3</v>
@@ -1818,27 +1810,27 @@
       </c>
       <c r="B18">
         <f t="shared" si="12"/>
-        <v>-10965</v>
+        <v>-10664</v>
       </c>
       <c r="C18">
         <f t="shared" si="12"/>
-        <v>32640</v>
+        <v>1024</v>
       </c>
       <c r="D18">
         <f>D$11*D7</f>
-        <v>-21675</v>
+        <v>-680</v>
       </c>
       <c r="E18">
         <f>SUM(B18:D18)</f>
-        <v>0</v>
+        <v>-10320</v>
       </c>
       <c r="F18">
         <f t="shared" ref="F18:F19" si="15">INT(E18/$F$1)</f>
-        <v>0</v>
+        <v>-41</v>
       </c>
       <c r="G18">
         <f>IF(F18+$F$2&gt;($F$1-1),$F$1-1,F18+$F$2)</f>
-        <v>128</v>
+        <v>87</v>
       </c>
       <c r="I18" t="s">
         <v>2</v>
@@ -1853,27 +1845,27 @@
       </c>
       <c r="L18">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>-10496</v>
       </c>
       <c r="M18">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>-8118</v>
       </c>
       <c r="N18">
         <f t="shared" si="16"/>
-        <v>65280</v>
+        <v>20480</v>
       </c>
       <c r="O18">
         <f t="shared" ref="O18:O19" si="17">SUM(J18:N18)</f>
-        <v>65280</v>
+        <v>1866</v>
       </c>
       <c r="P18">
         <f t="shared" ref="P18:P19" si="18">INT(O18/$F$1)</f>
-        <v>255</v>
+        <v>7</v>
       </c>
       <c r="Q18">
         <f t="shared" ref="Q18:Q19" si="19">IF(P18&gt;($F$1-2),$F$1-1,IF(P18&lt;0,0,P18))</f>
-        <v>255</v>
+        <v>7</v>
       </c>
       <c r="R18" t="s">
         <v>4</v>
@@ -1923,38 +1915,38 @@
       </c>
       <c r="B19">
         <f t="shared" si="12"/>
-        <v>32640</v>
+        <v>31744</v>
       </c>
       <c r="C19">
         <f t="shared" si="12"/>
-        <v>-5355</v>
+        <v>-168</v>
       </c>
       <c r="D19">
         <f>D$11*D8</f>
-        <v>-27285</v>
+        <v>-856</v>
       </c>
       <c r="E19">
         <f>SUM(B19:D19)</f>
-        <v>0</v>
+        <v>30720</v>
       </c>
       <c r="F19">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G19">
         <f>IF(F19+$F$2&gt;($F$1-1),$F$1-1,F19+$F$2)</f>
-        <v>128</v>
+        <v>248</v>
       </c>
       <c r="I19" t="s">
         <v>0</v>
       </c>
       <c r="J19">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>30720</v>
       </c>
       <c r="K19">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>12360</v>
       </c>
       <c r="L19">
         <f t="shared" si="16"/>
@@ -1966,19 +1958,19 @@
       </c>
       <c r="N19">
         <f t="shared" si="16"/>
-        <v>65280</v>
+        <v>20480</v>
       </c>
       <c r="O19">
         <f t="shared" si="17"/>
-        <v>65280</v>
+        <v>63560</v>
       </c>
       <c r="P19">
         <f t="shared" si="18"/>
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="Q19">
         <f t="shared" si="19"/>
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="R19" t="s">
         <v>5</v>
@@ -2025,15 +2017,15 @@
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="E20">
         <f>E18+32768</f>
-        <v>32768</v>
+        <v>22448</v>
       </c>
       <c r="K20">
         <f>J19+K19</f>
-        <v>0</v>
+        <v>43080</v>
       </c>
       <c r="M20">
         <f>L18+M18</f>
-        <v>0</v>
+        <v>-18614</v>
       </c>
       <c r="W20">
         <f>V19+W19</f>
@@ -2047,7 +2039,7 @@
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="E21">
         <f>E19+32768</f>
-        <v>32768</v>
+        <v>63488</v>
       </c>
       <c r="I21" t="s">
         <v>1</v>
@@ -2058,7 +2050,7 @@
       </c>
       <c r="K21" t="str">
         <f t="shared" ref="K21:P21" si="25">DEC2HEX(K17)</f>
-        <v>0</v>
+        <v>FFFFFFAA38</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" si="25"/>
@@ -2066,23 +2058,23 @@
       </c>
       <c r="M21" t="str">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>E18</v>
       </c>
       <c r="N21" t="str">
         <f t="shared" si="25"/>
-        <v>FF00</v>
+        <v>5000</v>
       </c>
       <c r="O21" t="str">
         <f t="shared" si="25"/>
-        <v>FF00</v>
+        <v>850</v>
       </c>
       <c r="P21" t="str">
         <f t="shared" si="25"/>
-        <v>FF</v>
+        <v>8</v>
       </c>
       <c r="Q21" t="str">
         <f t="shared" ref="Q21" si="26">DEC2HEX(Q17)</f>
-        <v>FF</v>
+        <v>8</v>
       </c>
       <c r="U21" t="s">
         <v>1</v>
@@ -2125,93 +2117,93 @@
         <v>3</v>
       </c>
       <c r="B22" t="str">
-        <f>DEC2HEX(B17)</f>
-        <v>4CB3</v>
+        <f t="shared" ref="B22:G24" si="28">DEC2HEX(B17)</f>
+        <v>4A98</v>
       </c>
       <c r="C22" t="str">
-        <f>DEC2HEX(C17)</f>
-        <v>1CE3</v>
+        <f t="shared" si="28"/>
+        <v>E8</v>
       </c>
       <c r="D22" t="str">
-        <f>DEC2HEX(D17)</f>
-        <v>956A</v>
+        <f t="shared" si="28"/>
+        <v>4B0</v>
       </c>
       <c r="E22" t="str">
-        <f>DEC2HEX(E17)</f>
-        <v>FF00</v>
+        <f t="shared" si="28"/>
+        <v>5030</v>
       </c>
       <c r="F22" t="str">
-        <f>DEC2HEX(F17)</f>
-        <v>FF</v>
+        <f t="shared" si="28"/>
+        <v>50</v>
       </c>
       <c r="G22" t="str">
-        <f>DEC2HEX(G17)</f>
-        <v>FF</v>
+        <f t="shared" si="28"/>
+        <v>50</v>
       </c>
       <c r="I22" t="s">
         <v>2</v>
       </c>
       <c r="J22" t="str">
-        <f t="shared" ref="J22:P24" si="28">DEC2HEX(J18)</f>
+        <f t="shared" ref="J22:P24" si="29">DEC2HEX(J18)</f>
         <v>0</v>
       </c>
       <c r="K22" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="L22" t="str">
-        <f t="shared" si="28"/>
-        <v>0</v>
+        <f t="shared" si="29"/>
+        <v>FFFFFFD700</v>
       </c>
       <c r="M22" t="str">
-        <f t="shared" si="28"/>
-        <v>0</v>
+        <f t="shared" si="29"/>
+        <v>FFFFFFE04A</v>
       </c>
       <c r="N22" t="str">
-        <f t="shared" si="28"/>
-        <v>FF00</v>
+        <f t="shared" si="29"/>
+        <v>5000</v>
       </c>
       <c r="O22" t="str">
-        <f t="shared" si="28"/>
-        <v>FF00</v>
+        <f t="shared" si="29"/>
+        <v>74A</v>
       </c>
       <c r="P22" t="str">
-        <f t="shared" si="28"/>
-        <v>FF</v>
+        <f t="shared" si="29"/>
+        <v>7</v>
       </c>
       <c r="Q22" t="str">
-        <f t="shared" ref="Q22" si="29">DEC2HEX(Q18)</f>
-        <v>FF</v>
+        <f t="shared" ref="Q22" si="30">DEC2HEX(Q18)</f>
+        <v>7</v>
       </c>
       <c r="U22" t="s">
         <v>2</v>
       </c>
       <c r="V22" t="str">
-        <f t="shared" ref="V22:AB22" si="30">DEC2HEX(V18)</f>
+        <f t="shared" ref="V22:AB22" si="31">DEC2HEX(V18)</f>
         <v>0</v>
       </c>
       <c r="W22" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="X22" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>FFFFFF9000</v>
       </c>
       <c r="Y22" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>FFFFFFA960</v>
       </c>
       <c r="Z22" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="AA22" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>FFFFFF3960</v>
       </c>
       <c r="AB22" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>FFFFFFFF39</v>
       </c>
       <c r="AC22" t="str">
@@ -2224,93 +2216,93 @@
         <v>4</v>
       </c>
       <c r="B23" t="str">
-        <f>DEC2HEX(B18)</f>
-        <v>FFFFFFD52B</v>
+        <f t="shared" si="28"/>
+        <v>FFFFFFD658</v>
       </c>
       <c r="C23" t="str">
-        <f>DEC2HEX(C18)</f>
-        <v>7F80</v>
+        <f t="shared" si="28"/>
+        <v>400</v>
       </c>
       <c r="D23" t="str">
-        <f>DEC2HEX(D18)</f>
-        <v>FFFFFFAB55</v>
+        <f t="shared" si="28"/>
+        <v>FFFFFFFD58</v>
       </c>
       <c r="E23" t="str">
-        <f>DEC2HEX(E18)</f>
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>FFFFFFD7B0</v>
       </c>
       <c r="F23" t="str">
-        <f>DEC2HEX(F18)</f>
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>FFFFFFFFD7</v>
       </c>
       <c r="G23" t="str">
-        <f>DEC2HEX(G18)</f>
-        <v>80</v>
+        <f t="shared" si="28"/>
+        <v>57</v>
       </c>
       <c r="I23" t="s">
         <v>0</v>
       </c>
       <c r="J23" t="str">
-        <f t="shared" si="28"/>
-        <v>0</v>
+        <f t="shared" si="29"/>
+        <v>7800</v>
       </c>
       <c r="K23" t="str">
-        <f t="shared" si="28"/>
-        <v>0</v>
+        <f t="shared" si="29"/>
+        <v>3048</v>
       </c>
       <c r="L23" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="M23" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="N23" t="str">
-        <f t="shared" si="28"/>
-        <v>FF00</v>
+        <f t="shared" si="29"/>
+        <v>5000</v>
       </c>
       <c r="O23" t="str">
-        <f t="shared" si="28"/>
-        <v>FF00</v>
+        <f t="shared" si="29"/>
+        <v>F848</v>
       </c>
       <c r="P23" t="str">
-        <f t="shared" si="28"/>
-        <v>FF</v>
+        <f t="shared" si="29"/>
+        <v>F8</v>
       </c>
       <c r="Q23" t="str">
-        <f t="shared" ref="Q23" si="31">DEC2HEX(Q19)</f>
-        <v>FF</v>
+        <f t="shared" ref="Q23" si="32">DEC2HEX(Q19)</f>
+        <v>F8</v>
       </c>
       <c r="U23" t="s">
         <v>0</v>
       </c>
       <c r="V23" t="str">
-        <f t="shared" ref="V23:AB23" si="32">DEC2HEX(V19)</f>
+        <f t="shared" ref="V23:AB23" si="33">DEC2HEX(V19)</f>
         <v>FFFFFF9000</v>
       </c>
       <c r="W23" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>FFFFFFD2F0</v>
       </c>
       <c r="X23" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="Y23" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="Z23" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AA23" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>FFFFFF62F0</v>
       </c>
       <c r="AB23" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>FFFFFFFF62</v>
       </c>
       <c r="AC23" t="str">
@@ -2323,273 +2315,273 @@
         <v>5</v>
       </c>
       <c r="B24" t="str">
-        <f>DEC2HEX(B19)</f>
-        <v>7F80</v>
+        <f t="shared" si="28"/>
+        <v>7C00</v>
       </c>
       <c r="C24" t="str">
-        <f>DEC2HEX(C19)</f>
-        <v>FFFFFFEB15</v>
+        <f t="shared" si="28"/>
+        <v>FFFFFFFF58</v>
       </c>
       <c r="D24" t="str">
-        <f>DEC2HEX(D19)</f>
-        <v>FFFFFF956B</v>
+        <f t="shared" si="28"/>
+        <v>FFFFFFFCA8</v>
       </c>
       <c r="E24" t="str">
-        <f>DEC2HEX(E19)</f>
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>7800</v>
       </c>
       <c r="F24" t="str">
-        <f>DEC2HEX(F19)</f>
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>78</v>
       </c>
       <c r="G24" t="str">
-        <f>DEC2HEX(G19)</f>
-        <v>80</v>
+        <f t="shared" si="28"/>
+        <v>F8</v>
       </c>
       <c r="K24" t="str">
-        <f t="shared" si="28"/>
-        <v>0</v>
+        <f t="shared" si="29"/>
+        <v>A848</v>
       </c>
       <c r="M24" t="str">
-        <f t="shared" si="28"/>
-        <v>0</v>
+        <f t="shared" si="29"/>
+        <v>FFFFFFB74A</v>
       </c>
       <c r="W24" t="str">
-        <f t="shared" ref="W24" si="33">DEC2HEX(W20)</f>
+        <f t="shared" ref="W24" si="34">DEC2HEX(W20)</f>
         <v>FFFFFF62F0</v>
       </c>
       <c r="Y24" t="str">
-        <f t="shared" ref="Y24" si="34">DEC2HEX(Y20)</f>
+        <f t="shared" ref="Y24" si="35">DEC2HEX(Y20)</f>
         <v>FFFFFF3960</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="E25" t="str">
-        <f t="shared" ref="E25:E26" si="35">DEC2HEX(E20)</f>
-        <v>8000</v>
+        <f t="shared" ref="E25:E26" si="36">DEC2HEX(E20)</f>
+        <v>57B0</v>
       </c>
       <c r="H25" t="str">
-        <f t="shared" ref="H25:Q25" si="36">DEC2HEX(-1*H17)</f>
+        <f t="shared" ref="H25:Q25" si="37">DEC2HEX(-1*H17)</f>
         <v>0</v>
       </c>
       <c r="J25" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="K25" t="str">
-        <f t="shared" si="36"/>
-        <v>0</v>
+        <f t="shared" si="37"/>
+        <v>55C8</v>
       </c>
       <c r="L25" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="M25" t="str">
-        <f t="shared" si="36"/>
-        <v>0</v>
+        <f t="shared" si="37"/>
+        <v>FFFFFFF1E8</v>
       </c>
       <c r="N25" t="str">
-        <f t="shared" si="36"/>
-        <v>FFFFFF0100</v>
+        <f t="shared" si="37"/>
+        <v>FFFFFFB000</v>
       </c>
       <c r="O25" t="str">
-        <f t="shared" si="36"/>
-        <v>FFFFFF0100</v>
+        <f t="shared" si="37"/>
+        <v>FFFFFFF7B0</v>
       </c>
       <c r="P25" t="str">
-        <f t="shared" si="36"/>
-        <v>FFFFFFFF01</v>
+        <f t="shared" si="37"/>
+        <v>FFFFFFFFF8</v>
       </c>
       <c r="Q25" t="str">
-        <f t="shared" si="36"/>
-        <v>FFFFFFFF01</v>
+        <f t="shared" si="37"/>
+        <v>FFFFFFFFF8</v>
       </c>
       <c r="T25" t="str">
-        <f t="shared" ref="T25" si="37">DEC2HEX(-1*T17)</f>
+        <f t="shared" ref="T25" si="38">DEC2HEX(-1*T17)</f>
         <v>0</v>
       </c>
       <c r="V25" t="str">
-        <f t="shared" ref="V25:AC25" si="38">DEC2HEX(-1*V17)</f>
+        <f t="shared" ref="V25:AC25" si="39">DEC2HEX(-1*V17)</f>
         <v>0</v>
       </c>
       <c r="W25" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>FFFFFFAFF0</v>
       </c>
       <c r="X25" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y25" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>FFFFFFD980</v>
       </c>
       <c r="Z25" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AA25" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>FFFFFF8970</v>
       </c>
       <c r="AB25" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>FFFFFFFF8A</v>
       </c>
       <c r="AC25" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>FFFFFFFF8A</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="E26" t="str">
-        <f t="shared" si="35"/>
-        <v>8000</v>
+        <f t="shared" si="36"/>
+        <v>F800</v>
       </c>
       <c r="H26" t="str">
-        <f t="shared" ref="H26:Q26" si="39">DEC2HEX(-1*H18)</f>
+        <f t="shared" ref="H26:Q26" si="40">DEC2HEX(-1*H18)</f>
         <v>0</v>
       </c>
       <c r="J26" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="K26" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="L26" t="str">
-        <f t="shared" si="39"/>
-        <v>0</v>
+        <f t="shared" si="40"/>
+        <v>2900</v>
       </c>
       <c r="M26" t="str">
-        <f t="shared" si="39"/>
-        <v>0</v>
+        <f t="shared" si="40"/>
+        <v>1FB6</v>
       </c>
       <c r="N26" t="str">
-        <f t="shared" si="39"/>
-        <v>FFFFFF0100</v>
+        <f t="shared" si="40"/>
+        <v>FFFFFFB000</v>
       </c>
       <c r="O26" t="str">
-        <f t="shared" si="39"/>
-        <v>FFFFFF0100</v>
+        <f t="shared" si="40"/>
+        <v>FFFFFFF8B6</v>
       </c>
       <c r="P26" t="str">
-        <f t="shared" si="39"/>
-        <v>FFFFFFFF01</v>
+        <f t="shared" si="40"/>
+        <v>FFFFFFFFF9</v>
       </c>
       <c r="Q26" t="str">
-        <f t="shared" si="39"/>
-        <v>FFFFFFFF01</v>
+        <f t="shared" si="40"/>
+        <v>FFFFFFFFF9</v>
       </c>
       <c r="T26" t="str">
-        <f t="shared" ref="T26" si="40">DEC2HEX(-1*T18)</f>
+        <f t="shared" ref="T26" si="41">DEC2HEX(-1*T18)</f>
         <v>0</v>
       </c>
       <c r="V26" t="str">
-        <f t="shared" ref="V26:AC26" si="41">DEC2HEX(-1*V18)</f>
+        <f t="shared" ref="V26:AC26" si="42">DEC2HEX(-1*V18)</f>
         <v>0</v>
       </c>
       <c r="W26" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="X26" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>7000</v>
       </c>
       <c r="Y26" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>56A0</v>
       </c>
       <c r="Z26" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AA26" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>C6A0</v>
       </c>
       <c r="AB26" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>C7</v>
       </c>
       <c r="AC26" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="H27" t="str">
-        <f t="shared" ref="H27:Q27" si="42">DEC2HEX(-1*H19)</f>
+        <f t="shared" ref="H27:Q27" si="43">DEC2HEX(-1*H19)</f>
         <v>0</v>
       </c>
       <c r="J27" t="str">
-        <f t="shared" si="42"/>
-        <v>0</v>
+        <f t="shared" si="43"/>
+        <v>FFFFFF8800</v>
       </c>
       <c r="K27" t="str">
-        <f t="shared" si="42"/>
-        <v>0</v>
+        <f t="shared" si="43"/>
+        <v>FFFFFFCFB8</v>
       </c>
       <c r="L27" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="M27" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="N27" t="str">
-        <f t="shared" si="42"/>
-        <v>FFFFFF0100</v>
+        <f t="shared" si="43"/>
+        <v>FFFFFFB000</v>
       </c>
       <c r="O27" t="str">
-        <f t="shared" si="42"/>
-        <v>FFFFFF0100</v>
+        <f t="shared" si="43"/>
+        <v>FFFFFF07B8</v>
       </c>
       <c r="P27" t="str">
-        <f t="shared" si="42"/>
-        <v>FFFFFFFF01</v>
+        <f t="shared" si="43"/>
+        <v>FFFFFFFF08</v>
       </c>
       <c r="Q27" t="str">
-        <f t="shared" si="42"/>
-        <v>FFFFFFFF01</v>
+        <f t="shared" si="43"/>
+        <v>FFFFFFFF08</v>
       </c>
       <c r="T27" t="str">
-        <f t="shared" ref="T27" si="43">DEC2HEX(-1*T19)</f>
+        <f t="shared" ref="T27" si="44">DEC2HEX(-1*T19)</f>
         <v>0</v>
       </c>
       <c r="V27" t="str">
-        <f t="shared" ref="V27:AC27" si="44">DEC2HEX(-1*V19)</f>
+        <f t="shared" ref="V27:AC27" si="45">DEC2HEX(-1*V19)</f>
         <v>7000</v>
       </c>
       <c r="W27" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>2D10</v>
       </c>
       <c r="X27" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="Y27" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="Z27" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AA27" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>9D10</v>
       </c>
       <c r="AB27" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>9E</v>
       </c>
       <c r="AC27" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
     </row>
@@ -2602,8 +2594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6249159-9F39-4AFA-B02F-9986699ECC31}">
   <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2682,7 +2674,7 @@
       </c>
       <c r="K2">
         <f>HEX2DEC(H2)</f>
-        <v>31</v>
+        <v>248</v>
       </c>
       <c r="L2">
         <f t="shared" ref="L2:M17" si="0">HEX2DEC(I2)</f>
@@ -2694,27 +2686,27 @@
       </c>
       <c r="O2">
         <f>INT( ( (K2*$B$8+L2*$C$8+M2*$D$8) /$E$1) +($E$1/2))</f>
-        <v>143</v>
+        <v>252</v>
       </c>
       <c r="P2">
         <f>INT(((K2*$B$7+L2*$C$7+M2*$D$7)/$E$1)+($E$1/2))</f>
-        <v>122</v>
+        <v>86</v>
       </c>
       <c r="Q2">
         <f>INT((K2*$B$6+L2*$C$6+M2*$D$6)/$E$1)</f>
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="S2" t="str">
         <f>DEC2HEX(IF(O2&lt;0,0,IF(O2&gt;($E$1-1),($E$1-1),O2)))</f>
-        <v>8F</v>
+        <v>FC</v>
       </c>
       <c r="T2" t="str">
         <f t="shared" ref="T2:U17" si="1">DEC2HEX(IF(P2&lt;0,0,IF(P2&gt;($E$1-1),($E$1-1),P2)))</f>
-        <v>7A</v>
+        <v>56</v>
       </c>
       <c r="U2" t="str">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>4A</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -2737,11 +2729,11 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K17" si="2">HEX2DEC(H3)</f>
-        <v>31</v>
+        <v>248</v>
       </c>
       <c r="L3">
         <f t="shared" si="0"/>
@@ -2749,31 +2741,31 @@
       </c>
       <c r="M3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="O3">
         <f t="shared" ref="O3:O17" si="3">INT( ( (K3*$B$8+L3*$C$8+M3*$D$8) /$E$1) +($E$1/2))</f>
-        <v>143</v>
+        <v>248</v>
       </c>
       <c r="P3">
         <f t="shared" ref="P3:P17" si="4">INT(((K3*$B$7+L3*$C$7+M3*$D$7)/$E$1)+($E$1/2))</f>
-        <v>122</v>
+        <v>83</v>
       </c>
       <c r="Q3">
         <f t="shared" ref="Q3:Q17" si="5">INT((K3*$B$6+L3*$C$6+M3*$D$6)/$E$1)</f>
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="S3" t="str">
         <f t="shared" ref="S3:S17" si="6">DEC2HEX(IF(O3&lt;0,0,IF(O3&gt;($E$1-1),($E$1-1),O3)))</f>
-        <v>8F</v>
+        <v>F8</v>
       </c>
       <c r="T3" t="str">
         <f t="shared" si="1"/>
-        <v>7A</v>
+        <v>53</v>
       </c>
       <c r="U3" t="str">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>4F</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -2796,11 +2788,11 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K4">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>248</v>
       </c>
       <c r="L4">
         <f t="shared" si="0"/>
@@ -2808,31 +2800,31 @@
       </c>
       <c r="M4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="O4">
         <f t="shared" si="3"/>
-        <v>142</v>
+        <v>245</v>
       </c>
       <c r="P4">
         <f t="shared" si="4"/>
-        <v>122</v>
+        <v>81</v>
       </c>
       <c r="Q4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>83</v>
       </c>
       <c r="S4" t="str">
         <f t="shared" si="6"/>
-        <v>8E</v>
+        <v>F5</v>
       </c>
       <c r="T4" t="str">
         <f t="shared" si="1"/>
-        <v>7A</v>
+        <v>51</v>
       </c>
       <c r="U4" t="str">
         <f t="shared" si="1"/>
-        <v>A</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -2843,11 +2835,11 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="K5">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>248</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
@@ -2855,31 +2847,31 @@
       </c>
       <c r="M5">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="O5">
         <f t="shared" si="3"/>
-        <v>142</v>
+        <v>241</v>
       </c>
       <c r="P5">
         <f t="shared" si="4"/>
-        <v>121</v>
+        <v>78</v>
       </c>
       <c r="Q5">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="S5" t="str">
         <f t="shared" si="6"/>
-        <v>8E</v>
+        <v>F1</v>
       </c>
       <c r="T5" t="str">
         <f t="shared" si="1"/>
-        <v>79</v>
+        <v>4E</v>
       </c>
       <c r="U5" t="str">
         <f t="shared" si="1"/>
-        <v>B</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -2905,11 +2897,11 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="K6">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>248</v>
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
@@ -2917,31 +2909,31 @@
       </c>
       <c r="M6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="O6">
         <f t="shared" si="3"/>
-        <v>141</v>
+        <v>238</v>
       </c>
       <c r="P6">
         <f t="shared" si="4"/>
-        <v>121</v>
+        <v>75</v>
       </c>
       <c r="Q6">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="S6" t="str">
         <f t="shared" si="6"/>
-        <v>8D</v>
+        <v>EE</v>
       </c>
       <c r="T6" t="str">
         <f t="shared" si="1"/>
-        <v>79</v>
+        <v>4B</v>
       </c>
       <c r="U6" t="str">
         <f t="shared" si="1"/>
-        <v>B</v>
+        <v>5D</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -2967,11 +2959,11 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="K7">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>248</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
@@ -2979,31 +2971,31 @@
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="O7">
         <f t="shared" si="3"/>
-        <v>141</v>
+        <v>235</v>
       </c>
       <c r="P7">
         <f t="shared" si="4"/>
-        <v>121</v>
+        <v>73</v>
       </c>
       <c r="Q7">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>98</v>
       </c>
       <c r="S7" t="str">
         <f t="shared" si="6"/>
-        <v>8D</v>
+        <v>EB</v>
       </c>
       <c r="T7" t="str">
         <f t="shared" si="1"/>
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="U7" t="str">
         <f t="shared" si="1"/>
-        <v>C</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -3029,11 +3021,11 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="K8">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>248</v>
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
@@ -3041,31 +3033,31 @@
       </c>
       <c r="M8">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="O8">
         <f t="shared" si="3"/>
-        <v>140</v>
+        <v>231</v>
       </c>
       <c r="P8">
         <f t="shared" si="4"/>
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="Q8">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="S8" t="str">
         <f t="shared" si="6"/>
-        <v>8C</v>
+        <v>E7</v>
       </c>
       <c r="T8" t="str">
         <f t="shared" si="1"/>
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="U8" t="str">
         <f t="shared" si="1"/>
-        <v>C</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -3076,11 +3068,11 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="K9">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>248</v>
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
@@ -3088,31 +3080,31 @@
       </c>
       <c r="M9">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="O9">
         <f t="shared" si="3"/>
-        <v>140</v>
+        <v>228</v>
       </c>
       <c r="P9">
         <f t="shared" si="4"/>
-        <v>120</v>
+        <v>67</v>
       </c>
       <c r="Q9">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>107</v>
       </c>
       <c r="S9" t="str">
         <f t="shared" si="6"/>
-        <v>8C</v>
+        <v>E4</v>
       </c>
       <c r="T9" t="str">
         <f t="shared" si="1"/>
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="U9" t="str">
         <f t="shared" si="1"/>
-        <v>D</v>
+        <v>6B</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -3123,11 +3115,11 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="K10">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>248</v>
       </c>
       <c r="L10">
         <f t="shared" si="0"/>
@@ -3135,31 +3127,31 @@
       </c>
       <c r="M10">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="O10">
         <f t="shared" si="3"/>
-        <v>140</v>
+        <v>225</v>
       </c>
       <c r="P10">
         <f t="shared" si="4"/>
-        <v>120</v>
+        <v>65</v>
       </c>
       <c r="Q10">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>112</v>
       </c>
       <c r="S10" t="str">
         <f t="shared" si="6"/>
-        <v>8C</v>
+        <v>E1</v>
       </c>
       <c r="T10" t="str">
         <f t="shared" si="1"/>
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="U10" t="str">
         <f t="shared" si="1"/>
-        <v>E</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -3170,11 +3162,11 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="K11">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>248</v>
       </c>
       <c r="L11">
         <f t="shared" si="0"/>
@@ -3182,31 +3174,31 @@
       </c>
       <c r="M11">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="O11">
         <f t="shared" si="3"/>
-        <v>139</v>
+        <v>221</v>
       </c>
       <c r="P11">
         <f t="shared" si="4"/>
-        <v>119</v>
+        <v>62</v>
       </c>
       <c r="Q11">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="S11" t="str">
         <f t="shared" si="6"/>
-        <v>8B</v>
+        <v>DD</v>
       </c>
       <c r="T11" t="str">
         <f t="shared" si="1"/>
-        <v>77</v>
+        <v>3E</v>
       </c>
       <c r="U11" t="str">
         <f t="shared" si="1"/>
-        <v>E</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -3216,12 +3208,12 @@
       <c r="I12">
         <v>0</v>
       </c>
-      <c r="J12" t="s">
-        <v>120</v>
+      <c r="J12">
+        <v>50</v>
       </c>
       <c r="K12">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>248</v>
       </c>
       <c r="L12">
         <f t="shared" si="0"/>
@@ -3229,31 +3221,31 @@
       </c>
       <c r="M12">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="O12">
         <f t="shared" si="3"/>
-        <v>139</v>
+        <v>218</v>
       </c>
       <c r="P12">
         <f t="shared" si="4"/>
-        <v>119</v>
+        <v>59</v>
       </c>
       <c r="Q12">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>121</v>
       </c>
       <c r="S12" t="str">
         <f t="shared" si="6"/>
-        <v>8B</v>
+        <v>DA</v>
       </c>
       <c r="T12" t="str">
         <f t="shared" si="1"/>
-        <v>77</v>
+        <v>3B</v>
       </c>
       <c r="U12" t="str">
         <f t="shared" si="1"/>
-        <v>F</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -3263,12 +3255,12 @@
       <c r="I13">
         <v>0</v>
       </c>
-      <c r="J13" t="s">
-        <v>2</v>
+      <c r="J13">
+        <v>58</v>
       </c>
       <c r="K13">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>248</v>
       </c>
       <c r="L13">
         <f t="shared" si="0"/>
@@ -3276,31 +3268,31 @@
       </c>
       <c r="M13">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="O13">
         <f t="shared" si="3"/>
-        <v>138</v>
+        <v>215</v>
       </c>
       <c r="P13">
         <f t="shared" si="4"/>
-        <v>119</v>
+        <v>57</v>
       </c>
       <c r="Q13">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>126</v>
       </c>
       <c r="S13" t="str">
         <f t="shared" si="6"/>
-        <v>8A</v>
+        <v>D7</v>
       </c>
       <c r="T13" t="str">
         <f t="shared" si="1"/>
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="U13" t="str">
         <f t="shared" si="1"/>
-        <v>F</v>
+        <v>7E</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -3310,12 +3302,12 @@
       <c r="I14">
         <v>0</v>
       </c>
-      <c r="J14" t="s">
-        <v>121</v>
+      <c r="J14">
+        <v>60</v>
       </c>
       <c r="K14">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>248</v>
       </c>
       <c r="L14">
         <f t="shared" si="0"/>
@@ -3323,31 +3315,31 @@
       </c>
       <c r="M14">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="O14">
         <f t="shared" si="3"/>
-        <v>138</v>
+        <v>211</v>
       </c>
       <c r="P14">
         <f t="shared" si="4"/>
-        <v>118</v>
+        <v>54</v>
       </c>
       <c r="Q14">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>130</v>
       </c>
       <c r="S14" t="str">
         <f t="shared" si="6"/>
-        <v>8A</v>
+        <v>D3</v>
       </c>
       <c r="T14" t="str">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>36</v>
       </c>
       <c r="U14" t="str">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -3357,12 +3349,12 @@
       <c r="I15">
         <v>0</v>
       </c>
-      <c r="J15" t="s">
-        <v>122</v>
+      <c r="J15">
+        <v>68</v>
       </c>
       <c r="K15">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>248</v>
       </c>
       <c r="L15">
         <f t="shared" si="0"/>
@@ -3370,31 +3362,31 @@
       </c>
       <c r="M15">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>104</v>
       </c>
       <c r="O15">
         <f t="shared" si="3"/>
-        <v>138</v>
+        <v>208</v>
       </c>
       <c r="P15">
         <f t="shared" si="4"/>
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="Q15">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>135</v>
       </c>
       <c r="S15" t="str">
         <f t="shared" si="6"/>
-        <v>8A</v>
+        <v>D0</v>
       </c>
       <c r="T15" t="str">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>33</v>
       </c>
       <c r="U15" t="str">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -3404,12 +3396,12 @@
       <c r="I16">
         <v>0</v>
       </c>
-      <c r="J16" t="s">
-        <v>123</v>
+      <c r="J16">
+        <v>70</v>
       </c>
       <c r="K16">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>248</v>
       </c>
       <c r="L16">
         <f t="shared" si="0"/>
@@ -3417,31 +3409,31 @@
       </c>
       <c r="M16">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>112</v>
       </c>
       <c r="O16">
         <f t="shared" si="3"/>
-        <v>137</v>
+        <v>205</v>
       </c>
       <c r="P16">
         <f t="shared" si="4"/>
-        <v>118</v>
+        <v>49</v>
       </c>
       <c r="Q16">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="S16" t="str">
         <f t="shared" si="6"/>
-        <v>89</v>
+        <v>CD</v>
       </c>
       <c r="T16" t="str">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="U16" t="str">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>8C</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -3451,12 +3443,12 @@
       <c r="I17">
         <v>0</v>
       </c>
-      <c r="J17" t="s">
-        <v>124</v>
+      <c r="J17">
+        <v>78</v>
       </c>
       <c r="K17">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>248</v>
       </c>
       <c r="L17">
         <f t="shared" si="0"/>
@@ -3464,31 +3456,31 @@
       </c>
       <c r="M17">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="O17">
         <f t="shared" si="3"/>
-        <v>137</v>
+        <v>201</v>
       </c>
       <c r="P17">
         <f t="shared" si="4"/>
-        <v>117</v>
+        <v>46</v>
       </c>
       <c r="Q17">
         <f t="shared" si="5"/>
-        <v>18</v>
+        <v>144</v>
       </c>
       <c r="S17" t="str">
         <f t="shared" si="6"/>
-        <v>89</v>
+        <v>C9</v>
       </c>
       <c r="T17" t="str">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>2E</v>
       </c>
       <c r="U17" t="str">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -3565,43 +3557,43 @@
       </c>
       <c r="H20" t="str">
         <f>S2</f>
-        <v>8F</v>
+        <v>FC</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" ref="I20:J35" si="9">T2</f>
-        <v>7A</v>
+        <v>56</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="9"/>
-        <v>9</v>
+        <v>4A</v>
       </c>
       <c r="K20">
         <f>HEX2DEC(H20)</f>
-        <v>143</v>
+        <v>252</v>
       </c>
       <c r="L20">
         <f>HEX2DEC(I20)</f>
-        <v>122</v>
+        <v>86</v>
       </c>
       <c r="M20">
         <f t="shared" ref="M20:M35" si="10">HEX2DEC(J20)</f>
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="O20">
         <f>INT((  (K20-($E$1/2))*$B$26+(K20-($E$1/2))*$C$26+(L20-($E$1/2))*$D$26+(L20-($E$1/2))*$E$26+M20*$F$26)/$E$1)</f>
-        <v>30</v>
+        <v>247</v>
       </c>
       <c r="P20">
-        <f>INT(((K20-($E$1/2))*$B$25+(K20-($E$1/2))*$C$25+(L20-($E$1/2))*$D$25+(L20-($E$1/2))*$E$25+M20*$F$25)/$E$1)</f>
-        <v>-2</v>
+        <f t="shared" ref="P20:P35" si="11">INT(((K20-($E$1/2))*$B$25+(K20-($E$1/2))*$C$25+(L20-($E$1/2))*$D$25+(L20-($E$1/2))*$E$25+M20*$F$25)/$E$1)</f>
+        <v>-1</v>
       </c>
       <c r="Q20">
-        <f>INT(((K20-($E$1/2))*$B$24+(K20-($E$1/2))*$C$24+(L20-($E$1/2))*$D$24+(L20-($E$1/2))*$E$24+M20*$F$24)/$E$1)</f>
-        <v>0</v>
+        <f t="shared" ref="Q20:Q35" si="12">INT(((K20-($E$1/2))*$B$24+(K20-($E$1/2))*$C$24+(L20-($E$1/2))*$D$24+(L20-($E$1/2))*$E$24+M20*$F$24)/$E$1)</f>
+        <v>-1</v>
       </c>
       <c r="S20" t="str">
         <f>DEC2HEX(IF(O20&lt;0,0,IF(O20&gt;($E$1-1),($E$1-1),O20)))</f>
-        <v>1E</v>
+        <v>F7</v>
       </c>
       <c r="T20" t="str">
         <f>DEC2HEX(IF(P20&lt;0,0,IF(P20&gt;($E$1-1),($E$1-1),P20)))</f>
@@ -3632,52 +3624,52 @@
         <v>1</v>
       </c>
       <c r="H21" t="str">
-        <f t="shared" ref="H21:H35" si="11">S3</f>
-        <v>8F</v>
+        <f t="shared" ref="H21:H35" si="13">S3</f>
+        <v>F8</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" si="9"/>
-        <v>7A</v>
+        <v>53</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="9"/>
-        <v>9</v>
+        <v>4F</v>
       </c>
       <c r="K21">
-        <f t="shared" ref="K21:L35" si="12">HEX2DEC(H21)</f>
-        <v>143</v>
+        <f t="shared" ref="K21:L35" si="14">HEX2DEC(H21)</f>
+        <v>248</v>
       </c>
       <c r="L21">
-        <f t="shared" si="12"/>
-        <v>122</v>
+        <f t="shared" si="14"/>
+        <v>83</v>
       </c>
       <c r="M21">
         <f t="shared" si="10"/>
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="O21">
-        <f>INT(((K21-($E$1/2))*$B$26+(K21-($E$1/2))*$C$26+(L21-($E$1/2))*$D$26+(L21-($E$1/2))*$E$26+M21*$F$26)/$E$1)</f>
-        <v>30</v>
+        <f t="shared" ref="O21:O35" si="15">INT(((K21-($E$1/2))*$B$26+(K21-($E$1/2))*$C$26+(L21-($E$1/2))*$D$26+(L21-($E$1/2))*$E$26+M21*$F$26)/$E$1)</f>
+        <v>247</v>
       </c>
       <c r="P21">
-        <f>INT(((K21-($E$1/2))*$B$25+(K21-($E$1/2))*$C$25+(L21-($E$1/2))*$D$25+(L21-($E$1/2))*$E$25+M21*$F$25)/$E$1)</f>
-        <v>-2</v>
+        <f t="shared" si="11"/>
+        <v>-1</v>
       </c>
       <c r="Q21">
-        <f>INT(((K21-($E$1/2))*$B$24+(K21-($E$1/2))*$C$24+(L21-($E$1/2))*$D$24+(L21-($E$1/2))*$E$24+M21*$F$24)/$E$1)</f>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>8</v>
       </c>
       <c r="S21" t="str">
-        <f t="shared" ref="S21:S35" si="13">DEC2HEX(IF(O21&lt;0,0,IF(O21&gt;($E$1-1),($E$1-1),O21)))</f>
-        <v>1E</v>
+        <f t="shared" ref="S21:S35" si="16">DEC2HEX(IF(O21&lt;0,0,IF(O21&gt;($E$1-1),($E$1-1),O21)))</f>
+        <v>F7</v>
       </c>
       <c r="T21" t="str">
-        <f>DEC2HEX(IF(P21&lt;0,0,IF(P21&gt;($E$1-1),($E$1-1),P21)))</f>
+        <f t="shared" ref="T21:T35" si="17">DEC2HEX(IF(P21&lt;0,0,IF(P21&gt;($E$1-1),($E$1-1),P21)))</f>
         <v>0</v>
       </c>
       <c r="U21" t="str">
-        <f>DEC2HEX(IF(Q21&lt;0,0,IF(Q21&gt;($E$1-1),($E$1-1),Q21)))</f>
-        <v>0</v>
+        <f t="shared" ref="U21:U35" si="18">DEC2HEX(IF(Q21&lt;0,0,IF(Q21&gt;($E$1-1),($E$1-1),Q21)))</f>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
@@ -3700,102 +3692,102 @@
         <v>1</v>
       </c>
       <c r="H22" t="str">
-        <f t="shared" si="11"/>
-        <v>8E</v>
+        <f t="shared" si="13"/>
+        <v>F5</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" si="9"/>
-        <v>7A</v>
+        <v>51</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="9"/>
-        <v>A</v>
+        <v>53</v>
       </c>
       <c r="K22">
-        <f t="shared" si="12"/>
-        <v>142</v>
+        <f t="shared" si="14"/>
+        <v>245</v>
       </c>
       <c r="L22">
-        <f t="shared" si="12"/>
-        <v>122</v>
+        <f t="shared" si="14"/>
+        <v>81</v>
       </c>
       <c r="M22">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v>83</v>
       </c>
       <c r="O22">
-        <f>INT(((K22-($E$1/2))*$B$26+(K22-($E$1/2))*$C$26+(L22-($E$1/2))*$D$26+(L22-($E$1/2))*$E$26+M22*$F$26)/$E$1)</f>
-        <v>29</v>
+        <f t="shared" si="15"/>
+        <v>247</v>
       </c>
       <c r="P22">
-        <f>INT(((K22-($E$1/2))*$B$25+(K22-($E$1/2))*$C$25+(L22-($E$1/2))*$D$25+(L22-($E$1/2))*$E$25+M22*$F$25)/$E$1)</f>
+        <f t="shared" si="11"/>
         <v>-1</v>
       </c>
       <c r="Q22">
-        <f>INT(((K22-($E$1/2))*$B$24+(K22-($E$1/2))*$C$24+(L22-($E$1/2))*$D$24+(L22-($E$1/2))*$E$24+M22*$F$24)/$E$1)</f>
-        <v>2</v>
+        <f t="shared" si="12"/>
+        <v>15</v>
       </c>
       <c r="S22" t="str">
-        <f t="shared" si="13"/>
-        <v>1D</v>
+        <f t="shared" si="16"/>
+        <v>F7</v>
       </c>
       <c r="T22" t="str">
-        <f>DEC2HEX(IF(P22&lt;0,0,IF(P22&gt;($E$1-1),($E$1-1),P22)))</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="U22" t="str">
-        <f>DEC2HEX(IF(Q22&lt;0,0,IF(Q22&gt;($E$1-1),($E$1-1),Q22)))</f>
-        <v>2</v>
+        <f t="shared" si="18"/>
+        <v>F</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H23" t="str">
-        <f t="shared" si="11"/>
-        <v>8E</v>
+        <f t="shared" si="13"/>
+        <v>F1</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="9"/>
-        <v>79</v>
+        <v>4E</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="9"/>
-        <v>B</v>
+        <v>58</v>
       </c>
       <c r="K23">
-        <f t="shared" si="12"/>
-        <v>142</v>
+        <f t="shared" si="14"/>
+        <v>241</v>
       </c>
       <c r="L23">
-        <f t="shared" si="12"/>
-        <v>121</v>
+        <f t="shared" si="14"/>
+        <v>78</v>
       </c>
       <c r="M23">
         <f t="shared" si="10"/>
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="O23">
-        <f>INT(((K23-($E$1/2))*$B$26+(K23-($E$1/2))*$C$26+(L23-($E$1/2))*$D$26+(L23-($E$1/2))*$E$26+M23*$F$26)/$E$1)</f>
-        <v>30</v>
+        <f t="shared" si="15"/>
+        <v>246</v>
       </c>
       <c r="P23">
-        <f>INT(((K23-($E$1/2))*$B$25+(K23-($E$1/2))*$C$25+(L23-($E$1/2))*$D$25+(L23-($E$1/2))*$E$25+M23*$F$25)/$E$1)</f>
-        <v>-2</v>
+        <f t="shared" si="11"/>
+        <v>-1</v>
       </c>
       <c r="Q23">
-        <f>INT(((K23-($E$1/2))*$B$24+(K23-($E$1/2))*$C$24+(L23-($E$1/2))*$D$24+(L23-($E$1/2))*$E$24+M23*$F$24)/$E$1)</f>
-        <v>3</v>
+        <f t="shared" si="12"/>
+        <v>24</v>
       </c>
       <c r="S23" t="str">
-        <f t="shared" si="13"/>
-        <v>1E</v>
+        <f t="shared" si="16"/>
+        <v>F6</v>
       </c>
       <c r="T23" t="str">
-        <f>DEC2HEX(IF(P23&lt;0,0,IF(P23&gt;($E$1-1),($E$1-1),P23)))</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="U23" t="str">
-        <f>DEC2HEX(IF(Q23&lt;0,0,IF(Q23&gt;($E$1-1),($E$1-1),Q23)))</f>
-        <v>3</v>
+        <f t="shared" si="18"/>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
@@ -3807,68 +3799,68 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <f t="shared" ref="C24:F24" si="14">ROUND($E$1*C20,0)</f>
+        <f t="shared" ref="C24:F24" si="19">ROUND($E$1*C20,0)</f>
         <v>-183</v>
       </c>
       <c r="D24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="E24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>-88</v>
       </c>
       <c r="F24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>256</v>
       </c>
       <c r="H24" t="str">
-        <f t="shared" si="11"/>
-        <v>8D</v>
+        <f t="shared" si="13"/>
+        <v>EE</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="9"/>
-        <v>79</v>
+        <v>4B</v>
       </c>
       <c r="J24" t="str">
         <f t="shared" si="9"/>
-        <v>B</v>
+        <v>5D</v>
       </c>
       <c r="K24">
-        <f t="shared" si="12"/>
-        <v>141</v>
+        <f t="shared" si="14"/>
+        <v>238</v>
       </c>
       <c r="L24">
-        <f t="shared" si="12"/>
-        <v>121</v>
+        <f t="shared" si="14"/>
+        <v>75</v>
       </c>
       <c r="M24">
         <f t="shared" si="10"/>
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="O24">
-        <f>INT(((K24-($E$1/2))*$B$26+(K24-($E$1/2))*$C$26+(L24-($E$1/2))*$D$26+(L24-($E$1/2))*$E$26+M24*$F$26)/$E$1)</f>
-        <v>29</v>
+        <f t="shared" si="15"/>
+        <v>247</v>
       </c>
       <c r="P24">
-        <f>INT(((K24-($E$1/2))*$B$25+(K24-($E$1/2))*$C$25+(L24-($E$1/2))*$D$25+(L24-($E$1/2))*$E$25+M24*$F$25)/$E$1)</f>
-        <v>-2</v>
+        <f t="shared" si="11"/>
+        <v>-1</v>
       </c>
       <c r="Q24">
-        <f>INT(((K24-($E$1/2))*$B$24+(K24-($E$1/2))*$C$24+(L24-($E$1/2))*$D$24+(L24-($E$1/2))*$E$24+M24*$F$24)/$E$1)</f>
-        <v>4</v>
+        <f t="shared" si="12"/>
+        <v>32</v>
       </c>
       <c r="S24" t="str">
-        <f t="shared" si="13"/>
-        <v>1D</v>
+        <f t="shared" si="16"/>
+        <v>F7</v>
       </c>
       <c r="T24" t="str">
-        <f>DEC2HEX(IF(P24&lt;0,0,IF(P24&gt;($E$1-1),($E$1-1),P24)))</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="U24" t="str">
-        <f>DEC2HEX(IF(Q24&lt;0,0,IF(Q24&gt;($E$1-1),($E$1-1),Q24)))</f>
-        <v>4</v>
+        <f t="shared" si="18"/>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
@@ -3876,72 +3868,72 @@
         <v>2</v>
       </c>
       <c r="B25">
-        <f t="shared" ref="B25:F26" si="15">ROUND($E$1*B21,0)</f>
+        <f t="shared" ref="B25:F26" si="20">ROUND($E$1*B21,0)</f>
         <v>0</v>
       </c>
       <c r="C25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="D25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>256</v>
       </c>
       <c r="E25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>198</v>
       </c>
       <c r="F25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>256</v>
       </c>
       <c r="H25" t="str">
-        <f t="shared" si="11"/>
-        <v>8D</v>
+        <f t="shared" si="13"/>
+        <v>EB</v>
       </c>
       <c r="I25" t="str">
         <f t="shared" si="9"/>
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="J25" t="str">
         <f t="shared" si="9"/>
-        <v>C</v>
+        <v>62</v>
       </c>
       <c r="K25">
-        <f t="shared" si="12"/>
-        <v>141</v>
+        <f t="shared" si="14"/>
+        <v>235</v>
       </c>
       <c r="L25">
-        <f t="shared" si="12"/>
-        <v>121</v>
+        <f t="shared" si="14"/>
+        <v>73</v>
       </c>
       <c r="M25">
         <f t="shared" si="10"/>
-        <v>12</v>
+        <v>98</v>
       </c>
       <c r="O25">
-        <f>INT(((K25-($E$1/2))*$B$26+(K25-($E$1/2))*$C$26+(L25-($E$1/2))*$D$26+(L25-($E$1/2))*$E$26+M25*$F$26)/$E$1)</f>
-        <v>30</v>
+        <f t="shared" si="15"/>
+        <v>248</v>
       </c>
       <c r="P25">
-        <f>INT(((K25-($E$1/2))*$B$25+(K25-($E$1/2))*$C$25+(L25-($E$1/2))*$D$25+(L25-($E$1/2))*$E$25+M25*$F$25)/$E$1)</f>
-        <v>-1</v>
+        <f t="shared" si="11"/>
+        <v>0</v>
       </c>
       <c r="Q25">
-        <f>INT(((K25-($E$1/2))*$B$24+(K25-($E$1/2))*$C$24+(L25-($E$1/2))*$D$24+(L25-($E$1/2))*$E$24+M25*$F$24)/$E$1)</f>
-        <v>5</v>
+        <f t="shared" si="12"/>
+        <v>40</v>
       </c>
       <c r="S25" t="str">
-        <f t="shared" si="13"/>
-        <v>1E</v>
+        <f t="shared" si="16"/>
+        <v>F8</v>
       </c>
       <c r="T25" t="str">
-        <f>DEC2HEX(IF(P25&lt;0,0,IF(P25&gt;($E$1-1),($E$1-1),P25)))</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="U25" t="str">
-        <f>DEC2HEX(IF(Q25&lt;0,0,IF(Q25&gt;($E$1-1),($E$1-1),Q25)))</f>
-        <v>5</v>
+        <f t="shared" si="18"/>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
@@ -3949,525 +3941,526 @@
         <v>0</v>
       </c>
       <c r="B26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>256</v>
       </c>
       <c r="C26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>103</v>
       </c>
       <c r="D26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="E26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="F26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>256</v>
       </c>
       <c r="H26" t="str">
-        <f t="shared" si="11"/>
-        <v>8C</v>
+        <f t="shared" si="13"/>
+        <v>E7</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="9"/>
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="J26" t="str">
         <f t="shared" si="9"/>
-        <v>C</v>
+        <v>66</v>
       </c>
       <c r="K26">
+        <f t="shared" si="14"/>
+        <v>231</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="14"/>
+        <v>70</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="10"/>
+        <v>102</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="15"/>
+        <v>246</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="11"/>
+        <v>-1</v>
+      </c>
+      <c r="Q26">
         <f t="shared" si="12"/>
+        <v>48</v>
+      </c>
+      <c r="S26" t="str">
+        <f t="shared" si="16"/>
+        <v>F6</v>
+      </c>
+      <c r="T26" t="str">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="U26" t="str">
+        <f t="shared" si="18"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="H27" t="str">
+        <f t="shared" si="13"/>
+        <v>E4</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="9"/>
+        <v>43</v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" si="9"/>
+        <v>6B</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="14"/>
+        <v>228</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="14"/>
+        <v>67</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="10"/>
+        <v>107</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="15"/>
+        <v>247</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="11"/>
+        <v>-2</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="12"/>
+        <v>56</v>
+      </c>
+      <c r="S27" t="str">
+        <f t="shared" si="16"/>
+        <v>F7</v>
+      </c>
+      <c r="T27" t="str">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="U27" t="str">
+        <f t="shared" si="18"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="H28" t="str">
+        <f t="shared" si="13"/>
+        <v>E1</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="9"/>
+        <v>41</v>
+      </c>
+      <c r="J28" t="str">
+        <f t="shared" si="9"/>
+        <v>70</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="14"/>
+        <v>225</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="14"/>
+        <v>65</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="10"/>
+        <v>112</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="15"/>
+        <v>248</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="12"/>
+        <v>64</v>
+      </c>
+      <c r="S28" t="str">
+        <f t="shared" si="16"/>
+        <v>F8</v>
+      </c>
+      <c r="T28" t="str">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="U28" t="str">
+        <f t="shared" si="18"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="H29" t="str">
+        <f t="shared" si="13"/>
+        <v>DD</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="9"/>
+        <v>3E</v>
+      </c>
+      <c r="J29" t="str">
+        <f t="shared" si="9"/>
+        <v>74</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="14"/>
+        <v>221</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="14"/>
+        <v>62</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="10"/>
+        <v>116</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="15"/>
+        <v>246</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="11"/>
+        <v>-2</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="12"/>
+        <v>72</v>
+      </c>
+      <c r="S29" t="str">
+        <f t="shared" si="16"/>
+        <v>F6</v>
+      </c>
+      <c r="T29" t="str">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="U29" t="str">
+        <f t="shared" si="18"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="H30" t="str">
+        <f t="shared" si="13"/>
+        <v>DA</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="9"/>
+        <v>3B</v>
+      </c>
+      <c r="J30" t="str">
+        <f t="shared" si="9"/>
+        <v>79</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="14"/>
+        <v>218</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="14"/>
+        <v>59</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="10"/>
+        <v>121</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="15"/>
+        <v>247</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="11"/>
+        <v>-2</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="12"/>
+        <v>80</v>
+      </c>
+      <c r="S30" t="str">
+        <f t="shared" si="16"/>
+        <v>F7</v>
+      </c>
+      <c r="T30" t="str">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="U30" t="str">
+        <f t="shared" si="18"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="H31" t="str">
+        <f t="shared" si="13"/>
+        <v>D7</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="9"/>
+        <v>39</v>
+      </c>
+      <c r="J31" t="str">
+        <f t="shared" si="9"/>
+        <v>7E</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="14"/>
+        <v>215</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="14"/>
+        <v>57</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="10"/>
+        <v>126</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="15"/>
+        <v>248</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="12"/>
+        <v>88</v>
+      </c>
+      <c r="S31" t="str">
+        <f t="shared" si="16"/>
+        <v>F8</v>
+      </c>
+      <c r="T31" t="str">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="U31" t="str">
+        <f t="shared" si="18"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="H32" t="str">
+        <f t="shared" si="13"/>
+        <v>D3</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="9"/>
+        <v>36</v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" si="9"/>
+        <v>82</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="14"/>
+        <v>211</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="14"/>
+        <v>54</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="10"/>
+        <v>130</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="15"/>
+        <v>246</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="11"/>
+        <v>-2</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="12"/>
+        <v>96</v>
+      </c>
+      <c r="S32" t="str">
+        <f t="shared" si="16"/>
+        <v>F6</v>
+      </c>
+      <c r="T32" t="str">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="U32" t="str">
+        <f t="shared" si="18"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H33" t="str">
+        <f t="shared" si="13"/>
+        <v>D0</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="9"/>
+        <v>33</v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="9"/>
+        <v>87</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="14"/>
+        <v>208</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="14"/>
+        <v>51</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="10"/>
+        <v>135</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="15"/>
+        <v>247</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="11"/>
+        <v>-2</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="12"/>
+        <v>104</v>
+      </c>
+      <c r="S33" t="str">
+        <f t="shared" si="16"/>
+        <v>F7</v>
+      </c>
+      <c r="T33" t="str">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="U33" t="str">
+        <f t="shared" si="18"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H34" t="str">
+        <f t="shared" si="13"/>
+        <v>CD</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="9"/>
+        <v>31</v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" si="9"/>
+        <v>8C</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="14"/>
+        <v>205</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="14"/>
+        <v>49</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="10"/>
         <v>140</v>
       </c>
-      <c r="L26">
+      <c r="O34">
+        <f t="shared" si="15"/>
+        <v>247</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="11"/>
+        <v>-1</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="12"/>
+        <v>112</v>
+      </c>
+      <c r="S34" t="str">
+        <f t="shared" si="16"/>
+        <v>F7</v>
+      </c>
+      <c r="T34" t="str">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="U34" t="str">
+        <f t="shared" si="18"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H35" t="str">
+        <f t="shared" si="13"/>
+        <v>C9</v>
+      </c>
+      <c r="I35" t="str">
+        <f t="shared" si="9"/>
+        <v>2E</v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" si="9"/>
+        <v>90</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="14"/>
+        <v>201</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="14"/>
+        <v>46</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="10"/>
+        <v>144</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="15"/>
+        <v>246</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="11"/>
+        <v>-2</v>
+      </c>
+      <c r="Q35">
         <f t="shared" si="12"/>
         <v>120</v>
       </c>
-      <c r="M26">
-        <f t="shared" si="10"/>
-        <v>12</v>
-      </c>
-      <c r="O26">
-        <f>INT(((K26-($E$1/2))*$B$26+(K26-($E$1/2))*$C$26+(L26-($E$1/2))*$D$26+(L26-($E$1/2))*$E$26+M26*$F$26)/$E$1)</f>
-        <v>28</v>
-      </c>
-      <c r="P26">
-        <f>INT(((K26-($E$1/2))*$B$25+(K26-($E$1/2))*$C$25+(L26-($E$1/2))*$D$25+(L26-($E$1/2))*$E$25+M26*$F$25)/$E$1)</f>
-        <v>-3</v>
-      </c>
-      <c r="Q26">
-        <f>INT(((K26-($E$1/2))*$B$24+(K26-($E$1/2))*$C$24+(L26-($E$1/2))*$D$24+(L26-($E$1/2))*$E$24+M26*$F$24)/$E$1)</f>
-        <v>6</v>
-      </c>
-      <c r="S26" t="str">
-        <f t="shared" si="13"/>
-        <v>1C</v>
-      </c>
-      <c r="T26" t="str">
-        <f>DEC2HEX(IF(P26&lt;0,0,IF(P26&gt;($E$1-1),($E$1-1),P26)))</f>
-        <v>0</v>
-      </c>
-      <c r="U26" t="str">
-        <f>DEC2HEX(IF(Q26&lt;0,0,IF(Q26&gt;($E$1-1),($E$1-1),Q26)))</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="H27" t="str">
-        <f t="shared" si="11"/>
-        <v>8C</v>
-      </c>
-      <c r="I27" t="str">
-        <f t="shared" si="9"/>
+      <c r="S35" t="str">
+        <f t="shared" si="16"/>
+        <v>F6</v>
+      </c>
+      <c r="T35" t="str">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="U35" t="str">
+        <f t="shared" si="18"/>
         <v>78</v>
       </c>
-      <c r="J27" t="str">
-        <f t="shared" si="9"/>
-        <v>D</v>
-      </c>
-      <c r="K27">
-        <f t="shared" si="12"/>
-        <v>140</v>
-      </c>
-      <c r="L27">
-        <f t="shared" si="12"/>
-        <v>120</v>
-      </c>
-      <c r="M27">
-        <f t="shared" si="10"/>
-        <v>13</v>
-      </c>
-      <c r="O27">
-        <f>INT(((K27-($E$1/2))*$B$26+(K27-($E$1/2))*$C$26+(L27-($E$1/2))*$D$26+(L27-($E$1/2))*$E$26+M27*$F$26)/$E$1)</f>
-        <v>29</v>
-      </c>
-      <c r="P27">
-        <f>INT(((K27-($E$1/2))*$B$25+(K27-($E$1/2))*$C$25+(L27-($E$1/2))*$D$25+(L27-($E$1/2))*$E$25+M27*$F$25)/$E$1)</f>
-        <v>-2</v>
-      </c>
-      <c r="Q27">
-        <f>INT(((K27-($E$1/2))*$B$24+(K27-($E$1/2))*$C$24+(L27-($E$1/2))*$D$24+(L27-($E$1/2))*$E$24+M27*$F$24)/$E$1)</f>
-        <v>7</v>
-      </c>
-      <c r="S27" t="str">
-        <f t="shared" si="13"/>
-        <v>1D</v>
-      </c>
-      <c r="T27" t="str">
-        <f>DEC2HEX(IF(P27&lt;0,0,IF(P27&gt;($E$1-1),($E$1-1),P27)))</f>
-        <v>0</v>
-      </c>
-      <c r="U27" t="str">
-        <f>DEC2HEX(IF(Q27&lt;0,0,IF(Q27&gt;($E$1-1),($E$1-1),Q27)))</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="H28" t="str">
-        <f t="shared" si="11"/>
-        <v>8C</v>
-      </c>
-      <c r="I28" t="str">
-        <f t="shared" si="9"/>
-        <v>78</v>
-      </c>
-      <c r="J28" t="str">
-        <f t="shared" si="9"/>
-        <v>E</v>
-      </c>
-      <c r="K28">
-        <f t="shared" si="12"/>
-        <v>140</v>
-      </c>
-      <c r="L28">
-        <f t="shared" si="12"/>
-        <v>120</v>
-      </c>
-      <c r="M28">
-        <f t="shared" si="10"/>
-        <v>14</v>
-      </c>
-      <c r="O28">
-        <f>INT(((K28-($E$1/2))*$B$26+(K28-($E$1/2))*$C$26+(L28-($E$1/2))*$D$26+(L28-($E$1/2))*$E$26+M28*$F$26)/$E$1)</f>
-        <v>30</v>
-      </c>
-      <c r="P28">
-        <f>INT(((K28-($E$1/2))*$B$25+(K28-($E$1/2))*$C$25+(L28-($E$1/2))*$D$25+(L28-($E$1/2))*$E$25+M28*$F$25)/$E$1)</f>
-        <v>-1</v>
-      </c>
-      <c r="Q28">
-        <f>INT(((K28-($E$1/2))*$B$24+(K28-($E$1/2))*$C$24+(L28-($E$1/2))*$D$24+(L28-($E$1/2))*$E$24+M28*$F$24)/$E$1)</f>
-        <v>8</v>
-      </c>
-      <c r="S28" t="str">
-        <f t="shared" si="13"/>
-        <v>1E</v>
-      </c>
-      <c r="T28" t="str">
-        <f>DEC2HEX(IF(P28&lt;0,0,IF(P28&gt;($E$1-1),($E$1-1),P28)))</f>
-        <v>0</v>
-      </c>
-      <c r="U28" t="str">
-        <f>DEC2HEX(IF(Q28&lt;0,0,IF(Q28&gt;($E$1-1),($E$1-1),Q28)))</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="H29" t="str">
-        <f t="shared" si="11"/>
-        <v>8B</v>
-      </c>
-      <c r="I29" t="str">
-        <f t="shared" si="9"/>
-        <v>77</v>
-      </c>
-      <c r="J29" t="str">
-        <f t="shared" si="9"/>
-        <v>E</v>
-      </c>
-      <c r="K29">
-        <f t="shared" si="12"/>
-        <v>139</v>
-      </c>
-      <c r="L29">
-        <f t="shared" si="12"/>
-        <v>119</v>
-      </c>
-      <c r="M29">
-        <f t="shared" si="10"/>
-        <v>14</v>
-      </c>
-      <c r="O29">
-        <f>INT(((K29-($E$1/2))*$B$26+(K29-($E$1/2))*$C$26+(L29-($E$1/2))*$D$26+(L29-($E$1/2))*$E$26+M29*$F$26)/$E$1)</f>
-        <v>29</v>
-      </c>
-      <c r="P29">
-        <f>INT(((K29-($E$1/2))*$B$25+(K29-($E$1/2))*$C$25+(L29-($E$1/2))*$D$25+(L29-($E$1/2))*$E$25+M29*$F$25)/$E$1)</f>
-        <v>-2</v>
-      </c>
-      <c r="Q29">
-        <f>INT(((K29-($E$1/2))*$B$24+(K29-($E$1/2))*$C$24+(L29-($E$1/2))*$D$24+(L29-($E$1/2))*$E$24+M29*$F$24)/$E$1)</f>
-        <v>9</v>
-      </c>
-      <c r="S29" t="str">
-        <f t="shared" si="13"/>
-        <v>1D</v>
-      </c>
-      <c r="T29" t="str">
-        <f>DEC2HEX(IF(P29&lt;0,0,IF(P29&gt;($E$1-1),($E$1-1),P29)))</f>
-        <v>0</v>
-      </c>
-      <c r="U29" t="str">
-        <f>DEC2HEX(IF(Q29&lt;0,0,IF(Q29&gt;($E$1-1),($E$1-1),Q29)))</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="H30" t="str">
-        <f t="shared" si="11"/>
-        <v>8B</v>
-      </c>
-      <c r="I30" t="str">
-        <f t="shared" si="9"/>
-        <v>77</v>
-      </c>
-      <c r="J30" t="str">
-        <f t="shared" si="9"/>
-        <v>F</v>
-      </c>
-      <c r="K30">
-        <f t="shared" si="12"/>
-        <v>139</v>
-      </c>
-      <c r="L30">
-        <f t="shared" si="12"/>
-        <v>119</v>
-      </c>
-      <c r="M30">
-        <f t="shared" si="10"/>
-        <v>15</v>
-      </c>
-      <c r="O30">
-        <f>INT(((K30-($E$1/2))*$B$26+(K30-($E$1/2))*$C$26+(L30-($E$1/2))*$D$26+(L30-($E$1/2))*$E$26+M30*$F$26)/$E$1)</f>
-        <v>30</v>
-      </c>
-      <c r="P30">
-        <f>INT(((K30-($E$1/2))*$B$25+(K30-($E$1/2))*$C$25+(L30-($E$1/2))*$D$25+(L30-($E$1/2))*$E$25+M30*$F$25)/$E$1)</f>
-        <v>-1</v>
-      </c>
-      <c r="Q30">
-        <f>INT(((K30-($E$1/2))*$B$24+(K30-($E$1/2))*$C$24+(L30-($E$1/2))*$D$24+(L30-($E$1/2))*$E$24+M30*$F$24)/$E$1)</f>
-        <v>10</v>
-      </c>
-      <c r="S30" t="str">
-        <f t="shared" si="13"/>
-        <v>1E</v>
-      </c>
-      <c r="T30" t="str">
-        <f>DEC2HEX(IF(P30&lt;0,0,IF(P30&gt;($E$1-1),($E$1-1),P30)))</f>
-        <v>0</v>
-      </c>
-      <c r="U30" t="str">
-        <f>DEC2HEX(IF(Q30&lt;0,0,IF(Q30&gt;($E$1-1),($E$1-1),Q30)))</f>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="H31" t="str">
-        <f t="shared" si="11"/>
-        <v>8A</v>
-      </c>
-      <c r="I31" t="str">
-        <f t="shared" si="9"/>
-        <v>77</v>
-      </c>
-      <c r="J31" t="str">
-        <f t="shared" si="9"/>
-        <v>F</v>
-      </c>
-      <c r="K31">
-        <f t="shared" si="12"/>
-        <v>138</v>
-      </c>
-      <c r="L31">
-        <f t="shared" si="12"/>
-        <v>119</v>
-      </c>
-      <c r="M31">
-        <f t="shared" si="10"/>
-        <v>15</v>
-      </c>
-      <c r="O31">
-        <f>INT(((K31-($E$1/2))*$B$26+(K31-($E$1/2))*$C$26+(L31-($E$1/2))*$D$26+(L31-($E$1/2))*$E$26+M31*$F$26)/$E$1)</f>
-        <v>29</v>
-      </c>
-      <c r="P31">
-        <f>INT(((K31-($E$1/2))*$B$25+(K31-($E$1/2))*$C$25+(L31-($E$1/2))*$D$25+(L31-($E$1/2))*$E$25+M31*$F$25)/$E$1)</f>
-        <v>-1</v>
-      </c>
-      <c r="Q31">
-        <f>INT(((K31-($E$1/2))*$B$24+(K31-($E$1/2))*$C$24+(L31-($E$1/2))*$D$24+(L31-($E$1/2))*$E$24+M31*$F$24)/$E$1)</f>
-        <v>10</v>
-      </c>
-      <c r="S31" t="str">
-        <f t="shared" si="13"/>
-        <v>1D</v>
-      </c>
-      <c r="T31" t="str">
-        <f>DEC2HEX(IF(P31&lt;0,0,IF(P31&gt;($E$1-1),($E$1-1),P31)))</f>
-        <v>0</v>
-      </c>
-      <c r="U31" t="str">
-        <f>DEC2HEX(IF(Q31&lt;0,0,IF(Q31&gt;($E$1-1),($E$1-1),Q31)))</f>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="H32" t="str">
-        <f t="shared" si="11"/>
-        <v>8A</v>
-      </c>
-      <c r="I32" t="str">
-        <f t="shared" si="9"/>
-        <v>76</v>
-      </c>
-      <c r="J32" t="str">
-        <f t="shared" si="9"/>
-        <v>10</v>
-      </c>
-      <c r="K32">
-        <f t="shared" si="12"/>
-        <v>138</v>
-      </c>
-      <c r="L32">
-        <f t="shared" si="12"/>
-        <v>118</v>
-      </c>
-      <c r="M32">
-        <f t="shared" si="10"/>
-        <v>16</v>
-      </c>
-      <c r="O32">
-        <f>INT(((K32-($E$1/2))*$B$26+(K32-($E$1/2))*$C$26+(L32-($E$1/2))*$D$26+(L32-($E$1/2))*$E$26+M32*$F$26)/$E$1)</f>
-        <v>30</v>
-      </c>
-      <c r="P32">
-        <f>INT(((K32-($E$1/2))*$B$25+(K32-($E$1/2))*$C$25+(L32-($E$1/2))*$D$25+(L32-($E$1/2))*$E$25+M32*$F$25)/$E$1)</f>
-        <v>-2</v>
-      </c>
-      <c r="Q32">
-        <f>INT(((K32-($E$1/2))*$B$24+(K32-($E$1/2))*$C$24+(L32-($E$1/2))*$D$24+(L32-($E$1/2))*$E$24+M32*$F$24)/$E$1)</f>
-        <v>12</v>
-      </c>
-      <c r="S32" t="str">
-        <f t="shared" si="13"/>
-        <v>1E</v>
-      </c>
-      <c r="T32" t="str">
-        <f>DEC2HEX(IF(P32&lt;0,0,IF(P32&gt;($E$1-1),($E$1-1),P32)))</f>
-        <v>0</v>
-      </c>
-      <c r="U32" t="str">
-        <f>DEC2HEX(IF(Q32&lt;0,0,IF(Q32&gt;($E$1-1),($E$1-1),Q32)))</f>
-        <v>C</v>
-      </c>
-    </row>
-    <row r="33" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H33" t="str">
-        <f t="shared" si="11"/>
-        <v>8A</v>
-      </c>
-      <c r="I33" t="str">
-        <f t="shared" si="9"/>
-        <v>76</v>
-      </c>
-      <c r="J33" t="str">
-        <f t="shared" si="9"/>
-        <v>10</v>
-      </c>
-      <c r="K33">
-        <f t="shared" si="12"/>
-        <v>138</v>
-      </c>
-      <c r="L33">
-        <f t="shared" si="12"/>
-        <v>118</v>
-      </c>
-      <c r="M33">
-        <f t="shared" si="10"/>
-        <v>16</v>
-      </c>
-      <c r="O33">
-        <f>INT(((K33-($E$1/2))*$B$26+(K33-($E$1/2))*$C$26+(L33-($E$1/2))*$D$26+(L33-($E$1/2))*$E$26+M33*$F$26)/$E$1)</f>
-        <v>30</v>
-      </c>
-      <c r="P33">
-        <f>INT(((K33-($E$1/2))*$B$25+(K33-($E$1/2))*$C$25+(L33-($E$1/2))*$D$25+(L33-($E$1/2))*$E$25+M33*$F$25)/$E$1)</f>
-        <v>-2</v>
-      </c>
-      <c r="Q33">
-        <f>INT(((K33-($E$1/2))*$B$24+(K33-($E$1/2))*$C$24+(L33-($E$1/2))*$D$24+(L33-($E$1/2))*$E$24+M33*$F$24)/$E$1)</f>
-        <v>12</v>
-      </c>
-      <c r="S33" t="str">
-        <f t="shared" si="13"/>
-        <v>1E</v>
-      </c>
-      <c r="T33" t="str">
-        <f>DEC2HEX(IF(P33&lt;0,0,IF(P33&gt;($E$1-1),($E$1-1),P33)))</f>
-        <v>0</v>
-      </c>
-      <c r="U33" t="str">
-        <f>DEC2HEX(IF(Q33&lt;0,0,IF(Q33&gt;($E$1-1),($E$1-1),Q33)))</f>
-        <v>C</v>
-      </c>
-    </row>
-    <row r="34" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H34" t="str">
-        <f t="shared" si="11"/>
-        <v>89</v>
-      </c>
-      <c r="I34" t="str">
-        <f t="shared" si="9"/>
-        <v>76</v>
-      </c>
-      <c r="J34" t="str">
-        <f t="shared" si="9"/>
-        <v>11</v>
-      </c>
-      <c r="K34">
-        <f t="shared" si="12"/>
-        <v>137</v>
-      </c>
-      <c r="L34">
-        <f t="shared" si="12"/>
-        <v>118</v>
-      </c>
-      <c r="M34">
-        <f t="shared" si="10"/>
-        <v>17</v>
-      </c>
-      <c r="O34">
-        <f>INT(((K34-($E$1/2))*$B$26+(K34-($E$1/2))*$C$26+(L34-($E$1/2))*$D$26+(L34-($E$1/2))*$E$26+M34*$F$26)/$E$1)</f>
-        <v>29</v>
-      </c>
-      <c r="P34">
-        <f>INT(((K34-($E$1/2))*$B$25+(K34-($E$1/2))*$C$25+(L34-($E$1/2))*$D$25+(L34-($E$1/2))*$E$25+M34*$F$25)/$E$1)</f>
-        <v>-1</v>
-      </c>
-      <c r="Q34">
-        <f>INT(((K34-($E$1/2))*$B$24+(K34-($E$1/2))*$C$24+(L34-($E$1/2))*$D$24+(L34-($E$1/2))*$E$24+M34*$F$24)/$E$1)</f>
-        <v>14</v>
-      </c>
-      <c r="S34" t="str">
-        <f t="shared" si="13"/>
-        <v>1D</v>
-      </c>
-      <c r="T34" t="str">
-        <f>DEC2HEX(IF(P34&lt;0,0,IF(P34&gt;($E$1-1),($E$1-1),P34)))</f>
-        <v>0</v>
-      </c>
-      <c r="U34" t="str">
-        <f>DEC2HEX(IF(Q34&lt;0,0,IF(Q34&gt;($E$1-1),($E$1-1),Q34)))</f>
-        <v>E</v>
-      </c>
-    </row>
-    <row r="35" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H35" t="str">
-        <f t="shared" si="11"/>
-        <v>89</v>
-      </c>
-      <c r="I35" t="str">
-        <f t="shared" si="9"/>
-        <v>75</v>
-      </c>
-      <c r="J35" t="str">
-        <f t="shared" si="9"/>
-        <v>12</v>
-      </c>
-      <c r="K35">
-        <f t="shared" si="12"/>
-        <v>137</v>
-      </c>
-      <c r="L35">
-        <f t="shared" si="12"/>
-        <v>117</v>
-      </c>
-      <c r="M35">
-        <f t="shared" si="10"/>
-        <v>18</v>
-      </c>
-      <c r="O35">
-        <f>INT(((K35-($E$1/2))*$B$26+(K35-($E$1/2))*$C$26+(L35-($E$1/2))*$D$26+(L35-($E$1/2))*$E$26+M35*$F$26)/$E$1)</f>
-        <v>30</v>
-      </c>
-      <c r="P35">
-        <f>INT(((K35-($E$1/2))*$B$25+(K35-($E$1/2))*$C$25+(L35-($E$1/2))*$D$25+(L35-($E$1/2))*$E$25+M35*$F$25)/$E$1)</f>
-        <v>-2</v>
-      </c>
-      <c r="Q35">
-        <f>INT(((K35-($E$1/2))*$B$24+(K35-($E$1/2))*$C$24+(L35-($E$1/2))*$D$24+(L35-($E$1/2))*$E$24+M35*$F$24)/$E$1)</f>
-        <v>15</v>
-      </c>
-      <c r="S35" t="str">
-        <f t="shared" si="13"/>
-        <v>1E</v>
-      </c>
-      <c r="T35" t="str">
-        <f>DEC2HEX(IF(P35&lt;0,0,IF(P35&gt;($E$1-1),($E$1-1),P35)))</f>
-        <v>0</v>
-      </c>
-      <c r="U35" t="str">
-        <f>DEC2HEX(IF(Q35&lt;0,0,IF(Q35&gt;($E$1-1),($E$1-1),Q35)))</f>
-        <v>F</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>